<commit_message>
Add Behav Proc in press
</commit_message>
<xml_diff>
--- a/ENG corta/data/teaching-experience.xlsx
+++ b/ENG corta/data/teaching-experience.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1863B4-6A10-4AF3-BC2C-69A7403A1DAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFDFB82-2EE7-42E5-A56D-2582F6C1537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>what</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Cognition Module (leading research projects in psychoacoustics).</t>
   </si>
   <si>
-    <t>2017 - Present</t>
-  </si>
-  <si>
     <t>2015 - 2016</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>Research Lab II.</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
   </si>
 </sst>
 </file>
@@ -611,48 +611,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -930,22 +930,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,12 +962,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
+      <c r="B2" s="1">
+        <v>2019</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -976,15 +976,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>2017</v>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -993,129 +993,137 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
-        <v>2018</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+        <v>2017</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>2012</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2010</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1">
-        <v>2010</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E13" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>